<commit_message>
More files from ICE
Excel file that holds the data for communication build 
Communication build database 
Python file that connects with SQL database to allow user to add data manually (user input with input() function, and to 
avoid SQL injection, parameterized queries were implemented).
</commit_message>
<xml_diff>
--- a/communication_build.csv.xlsx
+++ b/communication_build.csv.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="14680"/>
+    <workbookView xWindow="-100" yWindow="460" windowWidth="25360" windowHeight="14560"/>
   </bookViews>
   <sheets>
     <sheet name="communication_build" sheetId="1" r:id="rId1"/>
@@ -622,7 +622,9 @@
   </sheetPr>
   <dimension ref="A1:AC16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>